<commit_message>
Fix(products): fix the sheet name and path create need fix data in xlsx
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Setembro" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,160 +436,155 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>DIA</t>
+          <t>F9</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>F9</t>
+          <t>F9PL</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>F9PL</t>
+          <t>F12</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>F12</t>
+          <t>F1269</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>F1269</t>
+          <t>F14</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>F14</t>
+          <t>F18</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F18</t>
+          <t>F18PL</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>F18PL</t>
+          <t>F24PL</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>F24PL</t>
+          <t>F1869</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>F1869</t>
+          <t>F9TB</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>F9TB</t>
+          <t>F9PLTB</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>F9PLTB</t>
+          <t>F12TB</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>F12TB</t>
+          <t>F1269TB</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>F1269TB</t>
+          <t>F14TB</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>F14TB</t>
+          <t>F18TB</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>F18TB</t>
+          <t>F18PLTB</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>F18PLTB</t>
+          <t>F24PLTB</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>F24PLTB</t>
+          <t>F1869TB</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>F1869TB</t>
+          <t>F9TC</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>F9TC</t>
+          <t>F9PLTC</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>F9PLTC</t>
+          <t>F12TC</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>F12TC</t>
+          <t>F1269TC</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>F1269TC</t>
+          <t>F14TC</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>F14TC</t>
+          <t>F18TC</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>F18TC</t>
+          <t>F18PLTC</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>F18PLTC</t>
+          <t>F24PLTC</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>F24PLTC</t>
+          <t>F1869TC</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>F1869TC</t>
+          <t>TOTAL3975</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL3975</t>
+          <t>TOTAL4575</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL4575</t>
+          <t>TOTAL4565</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>TOTAL4565</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>TOTAL4475</t>
         </is>

</xml_diff>

<commit_message>
FixedUp (products): xlsx data
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Setembro" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,159 +436,262 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>DIA</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>F9</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>F9PL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>F12</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>F1269</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>F14</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>F18</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>F18PL</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>F24PL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>F1869</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>F9TB</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>F9PLTB</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>F12TB</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>F1269TB</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>F14TB</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>F18TB</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>F18PLTB</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>F24PLTB</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>F1869TB</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>F9TC</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>F9PLTC</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>F12TC</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>F1269TC</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>F14TC</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>F18TC</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>F18PLTC</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>F24PLTC</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>F1869TC</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>TOTAL3975</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>TOTAL4575</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>TOTAL4565</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>TOTAL4475</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>7</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>5</v>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update(io): get delete update
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -704,6 +704,51 @@
       </c>
       <c r="AG3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>3</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>5</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed up (products): fix the name of column
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -581,22 +581,22 @@
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>3975</t>
+          <t>T3975</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>4575</t>
+          <t>T4575</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>4565</t>
+          <t>T4565</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>4475</t>
+          <t>T4475</t>
         </is>
       </c>
     </row>
@@ -615,11 +615,11 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="n">
+        <v>5</v>
+      </c>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>5</v>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
@@ -630,16 +630,16 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="n">
-        <v>5</v>
-      </c>
+      <c r="X2" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
       <c r="AD2" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>

</xml_diff>

<commit_message>
Fixedup(products): addnewline fix name colum error
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BV1"/>
+  <dimension ref="A1:BW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,371 +439,469 @@
           <t>DIA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr"/>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>RASCHEL</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>F9</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>F9PL</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>F12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>F1269</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>F14</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>F18</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>F18PL</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>F24PL</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>F1869</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>F9TB</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>F9PLTB</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>F12TB</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>F1269TB</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>F14TB</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>F18TB</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>F18PLTB</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>F24PLTB</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>F1869TB</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>F9TC</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>F9PLTC</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>F12TC</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>F1269TC</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>F14TC</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>F18TC</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>F18PLTC</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>F24PLTC</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>F1869TC</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>T3975</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>T4575</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>T4565</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>T4475</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">   </t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>JACQUARD</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>F7</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>F969</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>F1232</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>F1432</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>F7TB</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>F969TB</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>F1232TB</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>F1432TB</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>F7TC</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>F969TC</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>F1232TC</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>F1432TC</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL  </t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>T4496</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>T2760</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">  </t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>RASCHEL2</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="BB1" s="1" t="inlineStr">
-        <is>
-          <t>F12</t>
-        </is>
-      </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>F14</t>
+          <t xml:space="preserve">F9 </t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
         <is>
-          <t>F18</t>
+          <t xml:space="preserve">F12 </t>
         </is>
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>F9TB</t>
+          <t xml:space="preserve">F14 </t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>F12TB</t>
+          <t xml:space="preserve">F18 </t>
         </is>
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>F14TB</t>
+          <t xml:space="preserve">F9TB </t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
         <is>
-          <t>F18TB</t>
+          <t xml:space="preserve">F12TB </t>
         </is>
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>F9TC</t>
+          <t xml:space="preserve">F14TB </t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
         <is>
-          <t>F12TC</t>
+          <t xml:space="preserve">F18TB </t>
         </is>
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>F14TC</t>
+          <t xml:space="preserve">F9TC </t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
         <is>
-          <t>F18TC</t>
+          <t xml:space="preserve">F12TC </t>
         </is>
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve">F14TC </t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">F18TC </t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
           <t xml:space="preserve">TOTAL </t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
-        <is>
-          <t>T3975</t>
-        </is>
-      </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">T3975 </t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">    </t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>KETTEN</t>
         </is>
       </c>
-      <c r="BQ1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="BR1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>F24KET</t>
         </is>
       </c>
-      <c r="BS1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>F24KETTB</t>
         </is>
       </c>
-      <c r="BT1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>F24KETTC</t>
         </is>
       </c>
-      <c r="BU1" s="1" t="inlineStr">
+      <c r="BV1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL   </t>
         </is>
       </c>
-      <c r="BV1" s="1" t="inlineStr">
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>T2660</t>
         </is>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>12</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>5</v>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="n">
+        <v>5</v>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="n">
+        <v>3</v>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed up(enumsFinuras): return "DIA" in tablerows
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW2"/>
+  <dimension ref="A1:BW9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,11 @@
           <t>DIA</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>RASCHEL</t>
@@ -903,6 +907,603 @@
       <c r="BV2" t="inlineStr"/>
       <c r="BW2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="inlineStr"/>
+      <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
+      <c r="BS3" t="inlineStr"/>
+      <c r="BT3" t="inlineStr"/>
+      <c r="BU3" t="inlineStr"/>
+      <c r="BV3" t="inlineStr"/>
+      <c r="BW3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr"/>
+      <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
+      <c r="BS5" t="inlineStr"/>
+      <c r="BT5" t="inlineStr"/>
+      <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
+      <c r="BW5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
+      <c r="AS6" t="inlineStr"/>
+      <c r="AT6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU6" t="inlineStr"/>
+      <c r="AV6" t="inlineStr"/>
+      <c r="AW6" t="inlineStr"/>
+      <c r="AX6" t="inlineStr"/>
+      <c r="AY6" t="n">
+        <v>12</v>
+      </c>
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="inlineStr"/>
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="inlineStr"/>
+      <c r="BD6" t="inlineStr"/>
+      <c r="BE6" t="inlineStr"/>
+      <c r="BF6" t="inlineStr"/>
+      <c r="BG6" t="inlineStr"/>
+      <c r="BH6" t="inlineStr"/>
+      <c r="BI6" t="inlineStr"/>
+      <c r="BJ6" t="inlineStr"/>
+      <c r="BK6" t="inlineStr"/>
+      <c r="BL6" t="inlineStr"/>
+      <c r="BM6" t="inlineStr"/>
+      <c r="BN6" t="inlineStr"/>
+      <c r="BO6" t="inlineStr"/>
+      <c r="BP6" t="inlineStr"/>
+      <c r="BQ6" t="inlineStr"/>
+      <c r="BR6" t="inlineStr"/>
+      <c r="BS6" t="inlineStr"/>
+      <c r="BT6" t="inlineStr"/>
+      <c r="BU6" t="inlineStr"/>
+      <c r="BV6" t="inlineStr"/>
+      <c r="BW6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
+      <c r="AT7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU7" t="inlineStr"/>
+      <c r="AV7" t="inlineStr"/>
+      <c r="AW7" t="inlineStr"/>
+      <c r="AX7" t="inlineStr"/>
+      <c r="AY7" t="n">
+        <v>12</v>
+      </c>
+      <c r="AZ7" t="inlineStr"/>
+      <c r="BA7" t="inlineStr"/>
+      <c r="BB7" t="inlineStr"/>
+      <c r="BC7" t="inlineStr"/>
+      <c r="BD7" t="inlineStr"/>
+      <c r="BE7" t="inlineStr"/>
+      <c r="BF7" t="inlineStr"/>
+      <c r="BG7" t="inlineStr"/>
+      <c r="BH7" t="inlineStr"/>
+      <c r="BI7" t="inlineStr"/>
+      <c r="BJ7" t="inlineStr"/>
+      <c r="BK7" t="inlineStr"/>
+      <c r="BL7" t="inlineStr"/>
+      <c r="BM7" t="inlineStr"/>
+      <c r="BN7" t="inlineStr"/>
+      <c r="BO7" t="inlineStr"/>
+      <c r="BP7" t="inlineStr"/>
+      <c r="BQ7" t="inlineStr"/>
+      <c r="BR7" t="inlineStr"/>
+      <c r="BS7" t="inlineStr"/>
+      <c r="BT7" t="inlineStr"/>
+      <c r="BU7" t="inlineStr"/>
+      <c r="BV7" t="inlineStr"/>
+      <c r="BW7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
+      <c r="AB8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
+      <c r="AT8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU8" t="inlineStr"/>
+      <c r="AV8" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
+      <c r="AX8" t="inlineStr"/>
+      <c r="AY8" t="n">
+        <v>12</v>
+      </c>
+      <c r="AZ8" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
+      <c r="BB8" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
+      <c r="BD8" t="inlineStr"/>
+      <c r="BE8" t="inlineStr"/>
+      <c r="BF8" t="inlineStr"/>
+      <c r="BG8" t="inlineStr"/>
+      <c r="BH8" t="inlineStr"/>
+      <c r="BI8" t="inlineStr"/>
+      <c r="BJ8" t="inlineStr"/>
+      <c r="BK8" t="inlineStr"/>
+      <c r="BL8" t="inlineStr"/>
+      <c r="BM8" t="inlineStr"/>
+      <c r="BN8" t="inlineStr"/>
+      <c r="BO8" t="inlineStr"/>
+      <c r="BP8" t="inlineStr"/>
+      <c r="BQ8" t="inlineStr"/>
+      <c r="BR8" t="inlineStr"/>
+      <c r="BS8" t="inlineStr"/>
+      <c r="BT8" t="inlineStr"/>
+      <c r="BU8" t="inlineStr"/>
+      <c r="BV8" t="inlineStr"/>
+      <c r="BW8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>24</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS9" t="inlineStr"/>
+      <c r="AT9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU9" t="inlineStr"/>
+      <c r="AV9" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
+      <c r="AX9" t="inlineStr"/>
+      <c r="AY9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AZ9" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
+      <c r="BB9" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
+      <c r="BD9" t="inlineStr"/>
+      <c r="BE9" t="inlineStr"/>
+      <c r="BF9" t="inlineStr"/>
+      <c r="BG9" t="inlineStr"/>
+      <c r="BH9" t="inlineStr"/>
+      <c r="BI9" t="inlineStr"/>
+      <c r="BJ9" t="inlineStr"/>
+      <c r="BK9" t="inlineStr"/>
+      <c r="BL9" t="inlineStr"/>
+      <c r="BM9" t="inlineStr"/>
+      <c r="BN9" t="inlineStr"/>
+      <c r="BO9" t="inlineStr"/>
+      <c r="BP9" t="inlineStr"/>
+      <c r="BQ9" t="inlineStr"/>
+      <c r="BR9" t="inlineStr"/>
+      <c r="BS9" t="inlineStr"/>
+      <c r="BT9" t="inlineStr"/>
+      <c r="BU9" t="inlineStr"/>
+      <c r="BV9" t="inlineStr"/>
+      <c r="BW9" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>